<commit_message>
Megan and Ben played with modeling again after the dataset got more of the WBdata incorporated. Found zero-inflated poisson models.
</commit_message>
<xml_diff>
--- a/TEMPpubsbydiv.xlsx
+++ b/TEMPpubsbydiv.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPpubsbydiv" sheetId="1" r:id="rId1"/>
     <sheet name="DivTables" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -733,10 +733,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -793,6 +793,943 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TEMPpubsbydiv!$B$2:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>UNITED STATES</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CHINA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INDIA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GERMANY</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BRAZIL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>UNITED KINGDOM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FRANCE</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SPAIN</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>AUSTRALIA</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>JAPAN</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>ITALY</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>CANADA</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>MEXICO</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>SOUTH KOREA</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>BELGIUM</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>SWITZERLAND</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>SWEDEN</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>NETHERLANDS</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>DENMARK</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>CZECH REPUBLIC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TEMPpubsbydiv!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>885</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="770462208"/>
+        <c:axId val="770460248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="770462208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="770460248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="770460248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Author representation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="770462208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1060,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,610 +2044,610 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="C2">
-        <v>521</v>
+        <v>462</v>
       </c>
       <c r="D2">
-        <v>383</v>
+        <v>1227</v>
       </c>
       <c r="E2">
-        <v>53083</v>
+        <v>43551</v>
       </c>
       <c r="F2">
-        <v>69.36</v>
+        <v>68.650000000000006</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2">
-        <v>53566</v>
+        <v>48021</v>
       </c>
       <c r="I2">
-        <v>9.7263189336519399E-3</v>
+        <v>9.6207909039795099E-3</v>
       </c>
       <c r="J2">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="K2">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="L2">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>462</v>
+        <v>574</v>
       </c>
       <c r="D3">
-        <v>1227</v>
+        <v>885</v>
       </c>
       <c r="E3">
-        <v>43551</v>
+        <v>32073</v>
       </c>
       <c r="F3">
-        <v>68.650000000000006</v>
+        <v>68.22</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
       </c>
       <c r="H3">
-        <v>48021</v>
+        <v>32685</v>
       </c>
       <c r="I3">
-        <v>9.6207909039795099E-3</v>
+        <v>1.7561572586813502E-2</v>
       </c>
       <c r="J3">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="L3">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C4">
-        <v>92</v>
+        <v>388</v>
       </c>
       <c r="D4">
-        <v>293</v>
+        <v>431</v>
       </c>
       <c r="E4">
-        <v>34400</v>
+        <v>19824</v>
       </c>
       <c r="F4">
-        <v>67.86</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4">
-        <v>36632</v>
+        <v>20300</v>
       </c>
       <c r="I4">
-        <v>2.51146538545534E-3</v>
+        <v>1.9113300492610799E-2</v>
       </c>
       <c r="J4">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="K4">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="L4">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
       <c r="C5">
-        <v>402</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>139</v>
+        <v>423</v>
       </c>
       <c r="E5">
-        <v>35182</v>
+        <v>12531</v>
       </c>
       <c r="F5">
-        <v>67.510000000000005</v>
+        <v>67.91</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
       </c>
       <c r="H5">
-        <v>35587</v>
+        <v>14642</v>
       </c>
       <c r="I5">
-        <v>1.1296259870177299E-2</v>
+        <v>1.1610435732823401E-3</v>
       </c>
       <c r="J5">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="K5">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="L5">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>257</v>
+        <v>521</v>
       </c>
       <c r="D6">
-        <v>42</v>
+        <v>383</v>
       </c>
       <c r="E6">
-        <v>33172</v>
+        <v>53083</v>
       </c>
       <c r="F6">
-        <v>72.13</v>
+        <v>69.36</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H6">
-        <v>32736</v>
+        <v>53566</v>
       </c>
       <c r="I6">
-        <v>7.8506842619745793E-3</v>
+        <v>9.7263189336519399E-3</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K6">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="L6">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C7">
-        <v>574</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>885</v>
+        <v>379</v>
       </c>
       <c r="E7">
-        <v>32073</v>
+        <v>9837</v>
       </c>
       <c r="F7">
-        <v>68.22</v>
+        <v>70.75</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7">
-        <v>32685</v>
+        <v>11869</v>
       </c>
       <c r="I7">
-        <v>1.7561572586813502E-2</v>
+        <v>1.3480495408206301E-3</v>
       </c>
       <c r="J7">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K7">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="L7">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C8">
-        <v>427</v>
+        <v>35</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>313</v>
       </c>
       <c r="E8">
-        <v>27667</v>
+        <v>17134</v>
       </c>
       <c r="F8">
-        <v>73.45</v>
+        <v>66.959999999999994</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H8">
-        <v>27849</v>
+        <v>19288</v>
       </c>
       <c r="I8">
-        <v>1.5332686990556199E-2</v>
+        <v>1.8145997511406101E-3</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="K8">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C9">
-        <v>116</v>
+        <v>216</v>
       </c>
       <c r="D9">
-        <v>42</v>
+        <v>303</v>
       </c>
       <c r="E9">
-        <v>26105</v>
+        <v>17721</v>
       </c>
       <c r="F9">
-        <v>67.599999999999994</v>
+        <v>63.77</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9">
-        <v>26456</v>
+        <v>18705</v>
       </c>
       <c r="I9">
-        <v>4.3846386452978496E-3</v>
+        <v>1.15477145148356E-2</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="K9">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="L9">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>92</v>
+      </c>
+      <c r="D10">
+        <v>293</v>
+      </c>
+      <c r="E10">
+        <v>34400</v>
+      </c>
+      <c r="F10">
+        <v>67.86</v>
+      </c>
+      <c r="G10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <v>1856</v>
-      </c>
-      <c r="D10">
+      <c r="H10">
+        <v>36632</v>
+      </c>
+      <c r="I10">
+        <v>2.51146538545534E-3</v>
+      </c>
+      <c r="J10">
+        <v>14</v>
+      </c>
+      <c r="K10">
+        <v>29</v>
+      </c>
+      <c r="L10">
         <v>17</v>
-      </c>
-      <c r="E10">
-        <v>25463</v>
-      </c>
-      <c r="F10">
-        <v>74.45</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10">
-        <v>25256</v>
-      </c>
-      <c r="I10">
-        <v>7.3487488121634498E-2</v>
-      </c>
-      <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
-      </c>
-      <c r="L10">
-        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C11">
-        <v>388</v>
+        <v>44</v>
       </c>
       <c r="D11">
-        <v>431</v>
+        <v>292</v>
       </c>
       <c r="E11">
-        <v>19824</v>
+        <v>10994</v>
       </c>
       <c r="F11">
-        <v>70</v>
+        <v>74.709999999999994</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H11">
-        <v>20300</v>
+        <v>13033</v>
       </c>
       <c r="I11">
-        <v>1.9113300492610799E-2</v>
+        <v>3.3760454231565999E-3</v>
       </c>
       <c r="J11">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="K11">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L11">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C12">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D12">
-        <v>313</v>
+        <v>285</v>
       </c>
       <c r="E12">
-        <v>17134</v>
+        <v>8998</v>
       </c>
       <c r="F12">
-        <v>66.959999999999994</v>
+        <v>65.739999999999995</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
       </c>
       <c r="H12">
-        <v>19288</v>
+        <v>9934</v>
       </c>
       <c r="I12">
-        <v>1.8145997511406101E-3</v>
+        <v>7.1471713307831699E-3</v>
       </c>
       <c r="J12">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="K12">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L12">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>216</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>303</v>
+        <v>208</v>
       </c>
       <c r="E13">
-        <v>17721</v>
+        <v>12595</v>
       </c>
       <c r="F13">
-        <v>63.77</v>
+        <v>69.64</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H13">
-        <v>18705</v>
+        <v>14721</v>
       </c>
       <c r="I13">
-        <v>1.15477145148356E-2</v>
+        <v>6.7930167787514403E-4</v>
       </c>
       <c r="J13">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K13">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L13">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>721</v>
+        <v>402</v>
       </c>
       <c r="D14">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="E14">
-        <v>17101</v>
+        <v>35182</v>
       </c>
       <c r="F14">
-        <v>72.22</v>
+        <v>67.510000000000005</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H14">
-        <v>16602</v>
+        <v>35587</v>
       </c>
       <c r="I14">
-        <v>4.3428502590049399E-2</v>
+        <v>1.1296259870177299E-2</v>
       </c>
       <c r="J14">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L14">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C15">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="D15">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="E15">
-        <v>15937</v>
+        <v>4099</v>
       </c>
       <c r="F15">
-        <v>69.02</v>
+        <v>73.55</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H15">
-        <v>16091</v>
+        <v>4483</v>
       </c>
       <c r="I15">
-        <v>4.3502579081474103E-3</v>
+        <v>6.9150122685701504E-3</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>208</v>
+        <v>120</v>
       </c>
       <c r="E16">
-        <v>12595</v>
+        <v>4752</v>
       </c>
       <c r="F16">
-        <v>69.64</v>
+        <v>67.42</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H16">
-        <v>14721</v>
+        <v>5015</v>
       </c>
       <c r="I16">
-        <v>6.7930167787514403E-4</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K16">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L16">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C17">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>423</v>
+        <v>115</v>
       </c>
       <c r="E17">
-        <v>12531</v>
+        <v>6042</v>
       </c>
       <c r="F17">
-        <v>67.91</v>
+        <v>65.37</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
       <c r="H17">
-        <v>14642</v>
+        <v>7164</v>
       </c>
       <c r="I17">
-        <v>1.1610435732823401E-3</v>
+        <v>5.5834729201563395E-4</v>
       </c>
       <c r="J17">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="K17">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="L17">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1753,873 +2690,873 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C19">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>292</v>
+        <v>78</v>
       </c>
       <c r="E19">
-        <v>10994</v>
+        <v>9034</v>
       </c>
       <c r="F19">
-        <v>74.709999999999994</v>
+        <v>65.95</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H19">
-        <v>13033</v>
+        <v>9893</v>
       </c>
       <c r="I19">
-        <v>3.3760454231565999E-3</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="K19">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="L19">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="C20">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="E20">
-        <v>12554</v>
+        <v>4456</v>
       </c>
       <c r="F20">
-        <v>71.680000000000007</v>
+        <v>66.319999999999993</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H20">
-        <v>11905</v>
+        <v>5041</v>
       </c>
       <c r="I20">
-        <v>1.25997480050399E-2</v>
+        <v>1.98373338623289E-4</v>
       </c>
       <c r="J20">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K20">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="L20">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D21">
-        <v>379</v>
+        <v>72</v>
       </c>
       <c r="E21">
-        <v>9837</v>
+        <v>3147</v>
       </c>
       <c r="F21">
-        <v>70.75</v>
+        <v>67.02</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H21">
-        <v>11869</v>
+        <v>4075</v>
       </c>
       <c r="I21">
-        <v>1.3480495408206301E-3</v>
+        <v>2.4539877300613498E-3</v>
       </c>
       <c r="J21">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="K21">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="L21">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C22">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D22">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="E22">
-        <v>10211</v>
+        <v>4313</v>
       </c>
       <c r="F22">
-        <v>71</v>
+        <v>67.5</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H22">
-        <v>11678</v>
+        <v>5178</v>
       </c>
       <c r="I22">
-        <v>1.79825312553519E-3</v>
+        <v>1.9312475859405199E-3</v>
       </c>
       <c r="J22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K22">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L22">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D23">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E23">
-        <v>8906</v>
+        <v>15937</v>
       </c>
       <c r="F23">
-        <v>66.03</v>
+        <v>69.02</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H23">
-        <v>9958</v>
+        <v>16091</v>
       </c>
       <c r="I23">
-        <v>5.6236192006427002E-3</v>
+        <v>4.3502579081474103E-3</v>
       </c>
       <c r="J23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C24">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D24">
-        <v>285</v>
+        <v>55</v>
       </c>
       <c r="E24">
-        <v>8998</v>
+        <v>6330</v>
       </c>
       <c r="F24">
-        <v>65.739999999999995</v>
+        <v>68.09</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H24">
-        <v>9934</v>
+        <v>7594</v>
       </c>
       <c r="I24">
-        <v>7.1471713307831699E-3</v>
+        <v>1.06663155122465E-2</v>
       </c>
       <c r="J24">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="K24">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="L24">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="E25">
-        <v>9034</v>
+        <v>7339</v>
       </c>
       <c r="F25">
-        <v>65.95</v>
+        <v>60.09</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
       </c>
       <c r="H25">
-        <v>9893</v>
+        <v>6954</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>4.31406384814495E-4</v>
       </c>
       <c r="J25">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K25">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L25">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>48</v>
+      </c>
+      <c r="E26">
+        <v>10211</v>
+      </c>
+      <c r="F26">
+        <v>71</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26">
+        <v>11678</v>
+      </c>
+      <c r="I26">
+        <v>1.79825312553519E-3</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>9</v>
+      </c>
+      <c r="L26">
         <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26">
-        <v>13</v>
-      </c>
-      <c r="D26">
-        <v>47</v>
-      </c>
-      <c r="E26">
-        <v>7137</v>
-      </c>
-      <c r="F26">
-        <v>65.040000000000006</v>
-      </c>
-      <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26">
-        <v>8195</v>
-      </c>
-      <c r="I26">
-        <v>1.58633312995729E-3</v>
-      </c>
-      <c r="J26">
-        <v>6</v>
-      </c>
-      <c r="K26">
-        <v>15</v>
-      </c>
-      <c r="L26">
-        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D27">
         <v>47</v>
       </c>
       <c r="E27">
-        <v>8124</v>
+        <v>7137</v>
       </c>
       <c r="F27">
-        <v>75.56</v>
+        <v>65.040000000000006</v>
       </c>
       <c r="G27" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H27">
-        <v>7977</v>
+        <v>8195</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1.58633312995729E-3</v>
       </c>
       <c r="J27">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="K27">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L27">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C28">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E28">
-        <v>6330</v>
+        <v>8124</v>
       </c>
       <c r="F28">
-        <v>68.09</v>
+        <v>75.56</v>
       </c>
       <c r="G28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28">
+        <v>7977</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
         <v>12</v>
       </c>
-      <c r="H28">
-        <v>7594</v>
-      </c>
-      <c r="I28">
-        <v>1.06663155122465E-2</v>
-      </c>
-      <c r="J28">
-        <v>3</v>
-      </c>
       <c r="K28">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="L28">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D29">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E29">
-        <v>6042</v>
+        <v>3653</v>
       </c>
       <c r="F29">
-        <v>65.37</v>
+        <v>65.33</v>
       </c>
       <c r="G29" t="s">
         <v>14</v>
       </c>
       <c r="H29">
-        <v>7164</v>
+        <v>3543</v>
       </c>
       <c r="I29">
-        <v>5.5834729201563395E-4</v>
+        <v>2.5402201524132098E-3</v>
       </c>
       <c r="J29">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K29">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="L29">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>257</v>
       </c>
       <c r="D30">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E30">
-        <v>7339</v>
+        <v>33172</v>
       </c>
       <c r="F30">
-        <v>60.09</v>
+        <v>72.13</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H30">
-        <v>6954</v>
+        <v>32736</v>
       </c>
       <c r="I30">
-        <v>4.31406384814495E-4</v>
+        <v>7.8506842619745793E-3</v>
       </c>
       <c r="J30">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="K30">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="L30">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31">
+        <v>116</v>
+      </c>
+      <c r="D31">
         <v>42</v>
       </c>
-      <c r="C31">
-        <v>222</v>
-      </c>
-      <c r="D31">
-        <v>37</v>
-      </c>
       <c r="E31">
-        <v>7071</v>
+        <v>26105</v>
       </c>
       <c r="F31">
-        <v>69.36</v>
+        <v>67.599999999999994</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H31">
-        <v>6922</v>
+        <v>26456</v>
       </c>
       <c r="I31">
-        <v>3.2071655590869698E-2</v>
+        <v>4.3846386452978496E-3</v>
       </c>
       <c r="J31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K31">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="L31">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>721</v>
       </c>
       <c r="D32">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E32">
-        <v>5281</v>
+        <v>17101</v>
       </c>
       <c r="F32">
-        <v>64.27</v>
+        <v>72.22</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H32">
-        <v>6906</v>
+        <v>16602</v>
       </c>
       <c r="I32">
-        <v>4.3440486533449199E-4</v>
+        <v>4.3428502590049399E-2</v>
       </c>
       <c r="J32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K32">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C33">
-        <v>41</v>
+        <v>222</v>
       </c>
       <c r="D33">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E33">
-        <v>6712</v>
+        <v>7071</v>
       </c>
       <c r="F33">
-        <v>67.59</v>
+        <v>69.36</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H33">
-        <v>6196</v>
+        <v>6922</v>
       </c>
       <c r="I33">
-        <v>6.6171723692704998E-3</v>
+        <v>3.2071655590869698E-2</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K33">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D34">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E34">
-        <v>4313</v>
+        <v>6712</v>
       </c>
       <c r="F34">
-        <v>67.5</v>
+        <v>67.59</v>
       </c>
       <c r="G34" t="s">
         <v>14</v>
       </c>
       <c r="H34">
-        <v>5178</v>
+        <v>6196</v>
       </c>
       <c r="I34">
-        <v>1.9312475859405199E-3</v>
+        <v>6.6171723692704998E-3</v>
       </c>
       <c r="J34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K34">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L34">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="E35">
-        <v>4456</v>
+        <v>3424</v>
       </c>
       <c r="F35">
-        <v>66.319999999999993</v>
+        <v>64.739999999999995</v>
       </c>
       <c r="G35" t="s">
         <v>14</v>
       </c>
       <c r="H35">
-        <v>5041</v>
+        <v>4336</v>
       </c>
       <c r="I35">
-        <v>1.98373338623289E-4</v>
+        <v>4.6125461254612501E-4</v>
       </c>
       <c r="J35">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K35">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L35">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D36">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="E36">
-        <v>4752</v>
+        <v>2873</v>
       </c>
       <c r="F36">
-        <v>67.42</v>
+        <v>65.239999999999995</v>
       </c>
       <c r="G36" t="s">
         <v>14</v>
       </c>
       <c r="H36">
-        <v>5015</v>
+        <v>2703</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>2.5897151313355499E-3</v>
       </c>
       <c r="J36">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="K36">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="L36">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37">
-        <v>197</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E37">
-        <v>5061</v>
+        <v>5281</v>
       </c>
       <c r="F37">
-        <v>67.41</v>
+        <v>64.27</v>
       </c>
       <c r="G37" t="s">
         <v>14</v>
       </c>
       <c r="H37">
-        <v>4694</v>
+        <v>6906</v>
       </c>
       <c r="I37">
-        <v>4.1968470387729002E-2</v>
+        <v>4.3440486533449199E-4</v>
       </c>
       <c r="J37">
         <v>2</v>
       </c>
       <c r="K37">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C38">
-        <v>31</v>
+        <v>150</v>
       </c>
       <c r="D38">
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="E38">
-        <v>4099</v>
+        <v>12554</v>
       </c>
       <c r="F38">
-        <v>73.55</v>
+        <v>71.680000000000007</v>
       </c>
       <c r="G38" t="s">
         <v>23</v>
       </c>
       <c r="H38">
-        <v>4483</v>
+        <v>11905</v>
       </c>
       <c r="I38">
-        <v>6.9150122685701504E-3</v>
+        <v>1.25997480050399E-2</v>
       </c>
       <c r="J38">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="K38">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="L38">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C39">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D39">
         <v>28</v>
       </c>
       <c r="E39">
-        <v>4585</v>
+        <v>8906</v>
       </c>
       <c r="F39">
-        <v>64.72</v>
+        <v>66.03</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
       </c>
       <c r="H39">
-        <v>4434</v>
+        <v>9958</v>
       </c>
       <c r="I39">
-        <v>2.7063599458728E-3</v>
+        <v>5.6236192006427002E-3</v>
       </c>
       <c r="J39">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K39">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L39">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C40">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D40">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E40">
-        <v>4095</v>
+        <v>4585</v>
       </c>
       <c r="F40">
-        <v>66.08</v>
+        <v>64.72</v>
       </c>
       <c r="G40" t="s">
         <v>14</v>
       </c>
       <c r="H40">
-        <v>4394</v>
+        <v>4434</v>
       </c>
       <c r="I40">
-        <v>2.2758306781975402E-3</v>
+        <v>2.7063599458728E-3</v>
       </c>
       <c r="J40">
+        <v>6</v>
+      </c>
+      <c r="K40">
+        <v>7</v>
+      </c>
+      <c r="L40">
         <v>3</v>
-      </c>
-      <c r="K40">
-        <v>5</v>
-      </c>
-      <c r="L40">
-        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D41">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E41">
-        <v>3424</v>
+        <v>2818</v>
       </c>
       <c r="F41">
-        <v>64.739999999999995</v>
+        <v>64.040000000000006</v>
       </c>
       <c r="G41" t="s">
         <v>14</v>
       </c>
       <c r="H41">
-        <v>4336</v>
+        <v>2504</v>
       </c>
       <c r="I41">
-        <v>4.6125461254612501E-4</v>
+        <v>1.19808306709265E-3</v>
       </c>
       <c r="J41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K41">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="L41">
         <v>4</v>
@@ -2627,78 +3564,78 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C42">
         <v>10</v>
       </c>
       <c r="D42">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="E42">
-        <v>3147</v>
+        <v>4095</v>
       </c>
       <c r="F42">
-        <v>67.02</v>
+        <v>66.08</v>
       </c>
       <c r="G42" t="s">
         <v>14</v>
       </c>
       <c r="H42">
-        <v>4075</v>
+        <v>4394</v>
       </c>
       <c r="I42">
-        <v>2.4539877300613498E-3</v>
+        <v>2.2758306781975402E-3</v>
       </c>
       <c r="J42">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K42">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="L42">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C43">
-        <v>9</v>
+        <v>197</v>
       </c>
       <c r="D43">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E43">
-        <v>3653</v>
+        <v>5061</v>
       </c>
       <c r="F43">
-        <v>65.33</v>
+        <v>67.41</v>
       </c>
       <c r="G43" t="s">
         <v>14</v>
       </c>
       <c r="H43">
-        <v>3543</v>
+        <v>4694</v>
       </c>
       <c r="I43">
-        <v>2.5402201524132098E-3</v>
+        <v>4.1968470387729002E-2</v>
       </c>
       <c r="J43">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K43">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="L43">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2741,303 +3678,303 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45">
+        <v>58</v>
+      </c>
+      <c r="D45">
+        <v>19</v>
+      </c>
+      <c r="E45">
+        <v>2982</v>
+      </c>
+      <c r="F45">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="G45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45">
+        <v>2970</v>
+      </c>
+      <c r="I45">
+        <v>1.9528619528619499E-2</v>
+      </c>
+      <c r="J45">
+        <v>6</v>
+      </c>
+      <c r="K45">
+        <v>14</v>
+      </c>
+      <c r="L45">
         <v>7</v>
-      </c>
-      <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45">
-        <v>6</v>
-      </c>
-      <c r="D45">
-        <v>12</v>
-      </c>
-      <c r="E45">
-        <v>3623</v>
-      </c>
-      <c r="F45">
-        <v>64.45</v>
-      </c>
-      <c r="G45" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45">
-        <v>3390</v>
-      </c>
-      <c r="I45">
-        <v>1.76991150442478E-3</v>
-      </c>
-      <c r="J45">
-        <v>2</v>
-      </c>
-      <c r="K45">
-        <v>5</v>
-      </c>
-      <c r="L45">
-        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E46">
-        <v>2967</v>
+        <v>3022</v>
       </c>
       <c r="F46">
-        <v>65.47</v>
+        <v>64.319999999999993</v>
       </c>
       <c r="G46" t="s">
         <v>14</v>
       </c>
       <c r="H46">
-        <v>3296</v>
+        <v>2840</v>
       </c>
       <c r="I46">
-        <v>2.1237864077669902E-3</v>
+        <v>1.0563380281690101E-3</v>
       </c>
       <c r="J46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C47">
-        <v>17</v>
+        <v>1856</v>
       </c>
       <c r="D47">
         <v>17</v>
       </c>
       <c r="E47">
-        <v>3716</v>
+        <v>25463</v>
       </c>
       <c r="F47">
-        <v>67.319999999999993</v>
+        <v>74.45</v>
       </c>
       <c r="G47" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H47">
-        <v>3250</v>
+        <v>25256</v>
       </c>
       <c r="I47">
-        <v>5.2307692307692298E-3</v>
+        <v>7.3487488121634498E-2</v>
       </c>
       <c r="J47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K47">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L47">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C48">
+        <v>17</v>
+      </c>
+      <c r="D48">
+        <v>17</v>
+      </c>
+      <c r="E48">
+        <v>3716</v>
+      </c>
+      <c r="F48">
+        <v>67.319999999999993</v>
+      </c>
+      <c r="G48" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48">
+        <v>3250</v>
+      </c>
+      <c r="I48">
+        <v>5.2307692307692298E-3</v>
+      </c>
+      <c r="J48">
         <v>1</v>
       </c>
-      <c r="D48">
-        <v>14</v>
-      </c>
-      <c r="E48">
-        <v>1997</v>
-      </c>
-      <c r="F48">
-        <v>71.75</v>
-      </c>
-      <c r="G48" t="s">
-        <v>23</v>
-      </c>
-      <c r="H48">
-        <v>3142</v>
-      </c>
-      <c r="I48">
-        <v>3.1826861871419503E-4</v>
-      </c>
-      <c r="J48">
-        <v>4</v>
-      </c>
       <c r="K48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L48">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C49">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D49">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E49">
-        <v>2982</v>
+        <v>1804</v>
       </c>
       <c r="F49">
-        <v>72.900000000000006</v>
+        <v>73.31</v>
       </c>
       <c r="G49" t="s">
         <v>23</v>
       </c>
       <c r="H49">
-        <v>2970</v>
+        <v>1709</v>
       </c>
       <c r="I49">
-        <v>1.9528619528619499E-2</v>
+        <v>5.2662375658279704E-3</v>
       </c>
       <c r="J49">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K49">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L49">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
+        <v>23</v>
+      </c>
+      <c r="B50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50">
+        <v>427</v>
+      </c>
+      <c r="D50">
         <v>15</v>
       </c>
-      <c r="B50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C50">
-        <v>3</v>
-      </c>
-      <c r="D50">
-        <v>18</v>
-      </c>
       <c r="E50">
-        <v>3022</v>
+        <v>27667</v>
       </c>
       <c r="F50">
-        <v>64.319999999999993</v>
+        <v>73.45</v>
       </c>
       <c r="G50" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H50">
-        <v>2840</v>
+        <v>27849</v>
       </c>
       <c r="I50">
-        <v>1.0563380281690101E-3</v>
+        <v>1.5332686990556199E-2</v>
       </c>
       <c r="J50">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K50">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L50">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <v>7</v>
       </c>
       <c r="D51">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E51">
-        <v>2873</v>
+        <v>2967</v>
       </c>
       <c r="F51">
-        <v>65.239999999999995</v>
+        <v>65.47</v>
       </c>
       <c r="G51" t="s">
         <v>14</v>
       </c>
       <c r="H51">
-        <v>2703</v>
+        <v>3296</v>
       </c>
       <c r="I51">
-        <v>2.5897151313355499E-3</v>
+        <v>2.1237864077669902E-3</v>
       </c>
       <c r="J51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D52">
+        <v>14</v>
+      </c>
+      <c r="E52">
+        <v>1997</v>
+      </c>
+      <c r="F52">
+        <v>71.75</v>
+      </c>
+      <c r="G52" t="s">
         <v>23</v>
       </c>
-      <c r="E52">
-        <v>2818</v>
-      </c>
-      <c r="F52">
-        <v>64.040000000000006</v>
-      </c>
-      <c r="G52" t="s">
-        <v>14</v>
-      </c>
       <c r="H52">
-        <v>2504</v>
+        <v>3142</v>
       </c>
       <c r="I52">
-        <v>1.19808306709265E-3</v>
+        <v>3.1826861871419503E-4</v>
       </c>
       <c r="J52">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K52">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L52">
         <v>4</v>
@@ -3045,40 +3982,40 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C53">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D53">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E53">
-        <v>1804</v>
+        <v>3623</v>
       </c>
       <c r="F53">
-        <v>73.31</v>
+        <v>64.45</v>
       </c>
       <c r="G53" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H53">
-        <v>1709</v>
+        <v>3390</v>
       </c>
       <c r="I53">
-        <v>5.2662375658279704E-3</v>
+        <v>1.76991150442478E-3</v>
       </c>
       <c r="J53">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K53">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="L53">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3197,9 +4134,10 @@
     </row>
   </sheetData>
   <sortState ref="A2:L56">
-    <sortCondition descending="1" ref="H2:H56"/>
+    <sortCondition descending="1" ref="D2:D56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3207,7 +4145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -3219,36 +4157,36 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="B3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="I3" s="1" t="s">
+      <c r="F3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>